<commit_message>
VERSÃO FINAL PARA GITHUB
</commit_message>
<xml_diff>
--- a/RAMAL.xlsx
+++ b/RAMAL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\chatboot HRB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6856C421-A6B7-4D41-ACDD-7942AEC20B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D3902F-BA87-4989-AB89-59917A1E28BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BD91861-E993-4C8F-BFD4-8F543CDBB1A3}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BD91861-E993-4C8F-BFD4-8F543CDBB1A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,136 +34,139 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
-  <si>
-    <t xml:space="preserve">ALMOXARIFADO </t>
-  </si>
-  <si>
-    <t>AMBULATORIO</t>
-  </si>
-  <si>
-    <t>QUALIDADE</t>
-  </si>
-  <si>
-    <t>ASSISTÊNCIA SOCIAL</t>
-  </si>
-  <si>
-    <t>BIOIMAGEM</t>
-  </si>
-  <si>
-    <t>CENTRO CIRÚRGICO</t>
-  </si>
-  <si>
-    <t>CLASSIFICAÇÃO DE RISCO</t>
-  </si>
-  <si>
-    <t>CLINICA CIRURGICA</t>
-  </si>
-  <si>
-    <t>CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>CLINICA OBSTÉTRICA</t>
-  </si>
-  <si>
-    <t>CME</t>
-  </si>
-  <si>
-    <t>CONFORTO MÉDICO</t>
-  </si>
-  <si>
-    <t>COORDENAÇÃO ADM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COZINHA - SENUT </t>
-  </si>
-  <si>
-    <t>FARMÁCIA CENTRAL</t>
-  </si>
-  <si>
-    <t>FARMÁCIA EMERGENCIA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FARMÁCIA UTI </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FATURAMENTO </t>
-  </si>
-  <si>
-    <t>FISIOTERAPIA</t>
-  </si>
-  <si>
-    <t>GERENCIA OPERACIONAL</t>
-  </si>
-  <si>
-    <t>SESMT</t>
-  </si>
-  <si>
-    <t>INTER. CIRURGICO / NIR</t>
-  </si>
-  <si>
-    <t>LABORATORIO</t>
-  </si>
-  <si>
-    <t>LAVANDERIA</t>
-  </si>
-  <si>
-    <t>MANUTENÇÃO</t>
-  </si>
-  <si>
-    <t>NUTRIÇÃO</t>
-  </si>
-  <si>
-    <t>OUVIDORIA</t>
-  </si>
-  <si>
-    <t>PRESCRIÇÃO 1 - UTI</t>
-  </si>
-  <si>
-    <t>PRESCRIÇÃO 2 - UTI</t>
-  </si>
-  <si>
-    <t>MEDICO DIARISTA</t>
-  </si>
-  <si>
-    <t>RECEPÇÃO EMERGENCIA</t>
-  </si>
-  <si>
-    <t>RECEPÇÃO FISIOTERAPIA</t>
-  </si>
-  <si>
-    <t>RECEPÇÃO UTI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RECEPÇÃO PRINCIPAL </t>
-  </si>
-  <si>
-    <t>RH</t>
-  </si>
-  <si>
-    <t>SCIH / COORD. ENFERMAGEM</t>
-  </si>
-  <si>
-    <t>SECRETARIA ADM</t>
-  </si>
-  <si>
-    <t>SUPRIMENTOS</t>
-  </si>
-  <si>
-    <t>TI</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>SETOR</t>
   </si>
   <si>
     <t>RAMAL</t>
+  </si>
+  <si>
+    <t>aleatorio 1</t>
+  </si>
+  <si>
+    <t>aleatorio 2</t>
+  </si>
+  <si>
+    <t>aleatorio 3</t>
+  </si>
+  <si>
+    <t>aleatorio 4</t>
+  </si>
+  <si>
+    <t>aleatorio 5</t>
+  </si>
+  <si>
+    <t>aleatorio 6</t>
+  </si>
+  <si>
+    <t>aleatorio 7</t>
+  </si>
+  <si>
+    <t>aleatorio 8</t>
+  </si>
+  <si>
+    <t>aleatorio 9</t>
+  </si>
+  <si>
+    <t>aleatorio 10</t>
+  </si>
+  <si>
+    <t>aleatorio 11</t>
+  </si>
+  <si>
+    <t>aleatorio 12</t>
+  </si>
+  <si>
+    <t>aleatorio 13</t>
+  </si>
+  <si>
+    <t>aleatorio 14</t>
+  </si>
+  <si>
+    <t>aleatorio 15</t>
+  </si>
+  <si>
+    <t>aleatorio 16</t>
+  </si>
+  <si>
+    <t>aleatorio 17</t>
+  </si>
+  <si>
+    <t>aleatorio 18</t>
+  </si>
+  <si>
+    <t>aleatorio 19</t>
+  </si>
+  <si>
+    <t>aleatorio 20</t>
+  </si>
+  <si>
+    <t>aleatorio 21</t>
+  </si>
+  <si>
+    <t>aleatorio 22</t>
+  </si>
+  <si>
+    <t>aleatorio 23</t>
+  </si>
+  <si>
+    <t>aleatorio 24</t>
+  </si>
+  <si>
+    <t>aleatorio 25</t>
+  </si>
+  <si>
+    <t>aleatorio 26</t>
+  </si>
+  <si>
+    <t>aleatorio 27</t>
+  </si>
+  <si>
+    <t>aleatorio 28</t>
+  </si>
+  <si>
+    <t>aleatorio 29</t>
+  </si>
+  <si>
+    <t>aleatorio 30</t>
+  </si>
+  <si>
+    <t>aleatorio 31</t>
+  </si>
+  <si>
+    <t>aleatorio 32</t>
+  </si>
+  <si>
+    <t>aleatorio 33</t>
+  </si>
+  <si>
+    <t>aleatorio 34</t>
+  </si>
+  <si>
+    <t>aleatorio 35</t>
+  </si>
+  <si>
+    <t>aleatorio 36</t>
+  </si>
+  <si>
+    <t>aleatorio 37</t>
+  </si>
+  <si>
+    <t>aleatorio 38</t>
+  </si>
+  <si>
+    <t>aleatorio 39</t>
+  </si>
+  <si>
+    <t>aleatorio 40</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,6 +178,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -541,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{881991FC-2E05-4CFE-A620-61237AF5A849}">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,162 +565,162 @@
   <sheetData>
     <row r="1" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>213</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>218</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
         <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>224</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
         <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
         <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
         <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
         <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1">
         <v>8</v>
-      </c>
-      <c r="B9" s="1">
-        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1">
         <v>9</v>
-      </c>
-      <c r="B10" s="1">
-        <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1">
         <v>10</v>
-      </c>
-      <c r="B11" s="1">
-        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1">
         <v>11</v>
-      </c>
-      <c r="B12" s="1">
-        <v>229</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1">
         <v>12</v>
-      </c>
-      <c r="B13" s="1">
-        <v>240</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1">
         <v>13</v>
-      </c>
-      <c r="B14" s="1">
-        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1">
         <v>14</v>
-      </c>
-      <c r="B15" s="1">
-        <v>209</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1">
         <v>15</v>
-      </c>
-      <c r="B16" s="1">
-        <v>203</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1">
         <v>16</v>
-      </c>
-      <c r="B17" s="1">
-        <v>241</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="1">
         <v>17</v>
-      </c>
-      <c r="B18" s="1">
-        <v>214</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="1">
         <v>18</v>
-      </c>
-      <c r="B19" s="1">
-        <v>215</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1">
         <v>19</v>
-      </c>
-      <c r="B20" s="1">
-        <v>223</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -719,7 +728,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="1">
-        <v>226</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -727,7 +736,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="1">
-        <v>206</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -735,7 +744,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="1">
-        <v>237</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -743,71 +752,71 @@
         <v>24</v>
       </c>
       <c r="B24" s="1">
-        <v>242</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B25" s="1">
-        <v>229</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="1">
         <v>25</v>
-      </c>
-      <c r="B26" s="1">
-        <v>239</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="1">
         <v>26</v>
-      </c>
-      <c r="B27" s="1">
-        <v>220</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="1">
         <v>27</v>
-      </c>
-      <c r="B28" s="1">
-        <v>231</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="1">
         <v>28</v>
-      </c>
-      <c r="B29" s="1">
-        <v>232</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B30" s="1">
-        <v>219</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="1">
         <v>30</v>
-      </c>
-      <c r="B31" s="1">
-        <v>201</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="1">
         <v>31</v>
-      </c>
-      <c r="B32" s="1">
-        <v>216</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -815,63 +824,71 @@
         <v>33</v>
       </c>
       <c r="B33" s="1">
-        <v>205</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B34" s="1">
-        <v>233</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="1">
         <v>34</v>
-      </c>
-      <c r="B35" s="1">
-        <v>212</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="1">
         <v>35</v>
-      </c>
-      <c r="B36" s="1">
-        <v>221</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="1">
         <v>36</v>
-      </c>
-      <c r="B37" s="1">
-        <v>217</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="B38" s="1">
-        <v>238</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B39" s="1">
-        <v>230</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B40" s="1">
-        <v>225</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="1">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -879,6 +896,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A40">
     <sortCondition ref="A2:A40"/>
   </sortState>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>